<commit_message>
Deploying to gh-pages from  @ 1db5eabed9d8bd346b226250e4e057aaa0c0d7ac 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_2-3-3.xlsx
+++ b/assets/excel/2021_2-3-3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8185C069-54C2-4F0C-A248-B2C5C24B9D50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218F6E40-22D7-4DC5-9FF9-983A54A56A17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{3CE7386B-6119-47E1-99EF-197129A315DD}"/>
   </bookViews>
@@ -40,16 +40,10 @@
 Land</t>
   </si>
   <si>
-    <t>Anteil der Einbürgerungen an allen Ausländerinnen und Ausländer in Prozent</t>
-  </si>
-  <si>
     <t>Prozent</t>
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>Anteil der Einbürgerungen an allen Einwohnerinnen und Einwohner in Prozent</t>
   </si>
   <si>
     <t>Quelle: Einbürgerungsstatistik, Bevölkerungsfortschreibung, Ausländerzentralregister</t>
@@ -230,6 +224,12 @@
   </si>
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
+  </si>
+  <si>
+    <t>Anteil der Einbürgerungen an allen Einwohnerinnen und Einwohnern in Prozent</t>
+  </si>
+  <si>
+    <t>Anteil der Einbürgerungen an allen Ausländerinnen und Ausländern in Prozent</t>
   </si>
 </sst>
 </file>
@@ -456,6 +456,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,9 +478,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1096,7 +1096,7 @@
     <row r="1" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="S1" s="2"/>
     </row>
@@ -1106,7 +1106,7 @@
     <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
@@ -1127,7 +1127,7 @@
     <row r="4" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1184,34 +1184,34 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="34"/>
+      <c r="D7" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="35"/>
     </row>
     <row r="8" spans="2:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
-      <c r="C8" s="32"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="12">
         <v>2005</v>
       </c>
@@ -1262,30 +1262,30 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="30"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
-      <c r="S9" s="34"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="35"/>
     </row>
     <row r="10" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
@@ -1345,7 +1345,7 @@
         <v>101</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="20">
         <v>0.17979965181654728</v>
@@ -1402,7 +1402,7 @@
         <v>102</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" s="20">
         <v>0.16523401964242615</v>
@@ -1459,7 +1459,7 @@
         <v>103</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="20">
         <v>0.15264152344491291</v>
@@ -1516,7 +1516,7 @@
         <v>151</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" s="20">
         <v>0.10097091809376034</v>
@@ -1573,7 +1573,7 @@
         <v>153</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" s="20">
         <v>0.12017008689221668</v>
@@ -1630,7 +1630,7 @@
         <v>154</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="20">
         <v>4.0921134743066426E-2</v>
@@ -1687,7 +1687,7 @@
         <v>155</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="20">
         <v>7.7033199263753502E-2</v>
@@ -1744,7 +1744,7 @@
         <v>157</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" s="20">
         <v>0.16049813866741963</v>
@@ -1801,7 +1801,7 @@
         <v>158</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="20">
         <v>0.1146607622963783</v>
@@ -1858,7 +1858,7 @@
         <v>159</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D20" s="20">
         <v>0.12293240167582378</v>
@@ -1915,7 +1915,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D21" s="23">
         <v>0.12729977248422386</v>
@@ -1972,7 +1972,7 @@
         <v>241</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" s="20">
         <v>0.24899361388976762</v>
@@ -2029,7 +2029,7 @@
         <v>241001</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D23" s="20">
         <v>0.31120995716742711</v>
@@ -2086,7 +2086,7 @@
         <v>241999</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D24" s="20">
         <v>0.19663388891245959</v>
@@ -2143,7 +2143,7 @@
         <v>251</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D25" s="20">
         <v>0.12108671850353518</v>
@@ -2200,7 +2200,7 @@
         <v>252</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D26" s="20">
         <v>0.19269269269269271</v>
@@ -2257,7 +2257,7 @@
         <v>254</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D27" s="20">
         <v>0.19233217383525494</v>
@@ -2314,7 +2314,7 @@
         <v>255</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D28" s="20">
         <v>7.4437228881644807E-2</v>
@@ -2371,7 +2371,7 @@
         <v>256</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D29" s="20">
         <v>0.15412727417176453</v>
@@ -2428,7 +2428,7 @@
         <v>257</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D30" s="20">
         <v>0.13952898397530761</v>
@@ -2485,7 +2485,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" s="23">
         <v>0.20430524432753722</v>
@@ -2542,7 +2542,7 @@
         <v>351</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D32" s="20">
         <v>0.11729626625156211</v>
@@ -2599,7 +2599,7 @@
         <v>352</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D33" s="20">
         <v>8.9635417681560442E-2</v>
@@ -2656,7 +2656,7 @@
         <v>353</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D34" s="20">
         <v>0.12446914529808499</v>
@@ -2713,7 +2713,7 @@
         <v>354</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D35" s="20">
         <v>9.7367191151269666E-3</v>
@@ -2770,7 +2770,7 @@
         <v>355</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D36" s="20">
         <v>0.11228846164807542</v>
@@ -2827,7 +2827,7 @@
         <v>356</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D37" s="20">
         <v>5.2332336949290847E-2</v>
@@ -2884,7 +2884,7 @@
         <v>357</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D38" s="20">
         <v>5.2160727824109174E-2</v>
@@ -2941,7 +2941,7 @@
         <v>358</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D39" s="20">
         <v>0.10232831971292</v>
@@ -2998,7 +2998,7 @@
         <v>359</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D40" s="20">
         <v>0.15167324087033973</v>
@@ -3055,7 +3055,7 @@
         <v>360</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D41" s="20">
         <v>5.4672993604291314E-2</v>
@@ -3112,7 +3112,7 @@
         <v>361</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D42" s="20">
         <v>0.13200680170639301</v>
@@ -3169,7 +3169,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D43" s="23">
         <v>0.10093108929878127</v>
@@ -3226,7 +3226,7 @@
         <v>401</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D44" s="20">
         <v>0.26081458454080825</v>
@@ -3283,7 +3283,7 @@
         <v>402</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D45" s="20">
         <v>9.0921401350279527E-2</v>
@@ -3340,7 +3340,7 @@
         <v>403</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D46" s="20">
         <v>0.15451076845457698</v>
@@ -3397,7 +3397,7 @@
         <v>404</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D47" s="20">
         <v>0.28080628029350363</v>
@@ -3454,7 +3454,7 @@
         <v>405</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D48" s="20">
         <v>0.21902527767139027</v>
@@ -3511,7 +3511,7 @@
         <v>451</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D49" s="20">
         <v>7.8522059521446877E-2</v>
@@ -3568,7 +3568,7 @@
         <v>452</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D50" s="20">
         <v>0.10571825296642262</v>
@@ -3625,7 +3625,7 @@
         <v>453</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D51" s="20">
         <v>5.3327507999126202E-2</v>
@@ -3682,7 +3682,7 @@
         <v>454</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D52" s="20">
         <v>5.3210701478290039E-2</v>
@@ -3739,7 +3739,7 @@
         <v>455</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D53" s="20">
         <v>7.0011438488541786E-2</v>
@@ -3796,7 +3796,7 @@
         <v>456</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D54" s="20">
         <v>8.47949301557549E-2</v>
@@ -3853,7 +3853,7 @@
         <v>457</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D55" s="20">
         <v>7.5126017836370684E-2</v>
@@ -3910,7 +3910,7 @@
         <v>458</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D56" s="20">
         <v>7.2376740819686466E-2</v>
@@ -3967,7 +3967,7 @@
         <v>459</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D57" s="20">
         <v>4.6181794913882079E-2</v>
@@ -4024,7 +4024,7 @@
         <v>460</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D58" s="20">
         <v>0.21676573439777647</v>
@@ -4081,7 +4081,7 @@
         <v>461</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D59" s="20">
         <v>9.7092558015470787E-2</v>
@@ -4138,7 +4138,7 @@
         <v>462</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D60" s="20">
         <v>4.6588673775753181E-2</v>
@@ -4195,7 +4195,7 @@
         <v>4</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D61" s="23">
         <v>0.10680847471115458</v>
@@ -4252,7 +4252,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D62" s="23">
         <v>0.13617805274141206</v>
@@ -4313,34 +4313,34 @@
       <c r="B65" s="18"/>
     </row>
     <row r="67" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C67" s="31" t="s">
+      <c r="C67" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D67" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E67" s="33"/>
-      <c r="F67" s="33"/>
-      <c r="G67" s="33"/>
-      <c r="H67" s="33"/>
-      <c r="I67" s="33"/>
-      <c r="J67" s="33"/>
-      <c r="K67" s="33"/>
-      <c r="L67" s="33"/>
-      <c r="M67" s="33"/>
-      <c r="N67" s="33"/>
-      <c r="O67" s="33"/>
-      <c r="P67" s="33"/>
-      <c r="Q67" s="33"/>
-      <c r="R67" s="33"/>
-      <c r="S67" s="34"/>
+      <c r="D67" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E67" s="34"/>
+      <c r="F67" s="34"/>
+      <c r="G67" s="34"/>
+      <c r="H67" s="34"/>
+      <c r="I67" s="34"/>
+      <c r="J67" s="34"/>
+      <c r="K67" s="34"/>
+      <c r="L67" s="34"/>
+      <c r="M67" s="34"/>
+      <c r="N67" s="34"/>
+      <c r="O67" s="34"/>
+      <c r="P67" s="34"/>
+      <c r="Q67" s="34"/>
+      <c r="R67" s="34"/>
+      <c r="S67" s="35"/>
     </row>
     <row r="68" spans="2:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="29"/>
-      <c r="C68" s="32"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="33"/>
       <c r="D68" s="12">
         <v>2005</v>
       </c>
@@ -4391,80 +4391,80 @@
       </c>
     </row>
     <row r="69" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="30"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E69" s="33"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="33"/>
-      <c r="H69" s="33"/>
-      <c r="I69" s="33"/>
-      <c r="J69" s="33"/>
-      <c r="K69" s="33"/>
-      <c r="L69" s="33"/>
-      <c r="M69" s="33"/>
-      <c r="N69" s="33"/>
-      <c r="O69" s="33"/>
-      <c r="P69" s="33"/>
-      <c r="Q69" s="33"/>
-      <c r="R69" s="33"/>
-      <c r="S69" s="34"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="34"/>
+      <c r="H69" s="34"/>
+      <c r="I69" s="34"/>
+      <c r="J69" s="34"/>
+      <c r="K69" s="34"/>
+      <c r="L69" s="34"/>
+      <c r="M69" s="34"/>
+      <c r="N69" s="34"/>
+      <c r="O69" s="34"/>
+      <c r="P69" s="34"/>
+      <c r="Q69" s="34"/>
+      <c r="R69" s="34"/>
+      <c r="S69" s="35"/>
     </row>
     <row r="70" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="28">
+        <v>1</v>
+      </c>
+      <c r="D70" s="28">
+        <v>2</v>
+      </c>
+      <c r="E70" s="28">
+        <v>3</v>
+      </c>
+      <c r="F70" s="28">
         <v>4</v>
       </c>
-      <c r="C70" s="35">
-        <v>1</v>
-      </c>
-      <c r="D70" s="35">
-        <v>2</v>
-      </c>
-      <c r="E70" s="35">
-        <v>3</v>
-      </c>
-      <c r="F70" s="35">
-        <v>4</v>
-      </c>
-      <c r="G70" s="35">
+      <c r="G70" s="28">
         <v>5</v>
       </c>
-      <c r="H70" s="35">
+      <c r="H70" s="28">
         <v>6</v>
       </c>
-      <c r="I70" s="35">
+      <c r="I70" s="28">
         <v>7</v>
       </c>
-      <c r="J70" s="35">
+      <c r="J70" s="28">
         <v>8</v>
       </c>
-      <c r="K70" s="35">
+      <c r="K70" s="28">
         <v>9</v>
       </c>
-      <c r="L70" s="35">
+      <c r="L70" s="28">
         <v>10</v>
       </c>
-      <c r="M70" s="35">
+      <c r="M70" s="28">
         <v>11</v>
       </c>
-      <c r="N70" s="35">
+      <c r="N70" s="28">
         <v>12</v>
       </c>
-      <c r="O70" s="35">
+      <c r="O70" s="28">
         <v>13</v>
       </c>
-      <c r="P70" s="35">
+      <c r="P70" s="28">
         <v>14</v>
       </c>
-      <c r="Q70" s="35">
+      <c r="Q70" s="28">
         <v>15</v>
       </c>
-      <c r="R70" s="35">
+      <c r="R70" s="28">
         <v>16</v>
       </c>
-      <c r="S70" s="35">
+      <c r="S70" s="28">
         <v>17</v>
       </c>
     </row>
@@ -4474,7 +4474,7 @@
         <v>101</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D71" s="20">
         <v>2.1750924784217016</v>
@@ -4531,7 +4531,7 @@
         <v>102</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D72" s="20">
         <v>1.660292883126574</v>
@@ -4588,7 +4588,7 @@
         <v>103</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D73" s="20">
         <v>1.5434673786083766</v>
@@ -4645,7 +4645,7 @@
         <v>151</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D74" s="20">
         <v>2.3252758801891749</v>
@@ -4702,7 +4702,7 @@
         <v>153</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D75" s="20">
         <v>2.42472688515854</v>
@@ -4759,7 +4759,7 @@
         <v>154</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D76" s="20">
         <v>1.0964912280701753</v>
@@ -4816,7 +4816,7 @@
         <v>155</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D77" s="20">
         <v>1.9462624870823286</v>
@@ -4873,7 +4873,7 @@
         <v>157</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D78" s="20">
         <v>3.1606672519754171</v>
@@ -4930,7 +4930,7 @@
         <v>158</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D79" s="20">
         <v>2.9676627097830535</v>
@@ -4987,7 +4987,7 @@
         <v>159</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D80" s="20">
         <v>2.0925871088737535</v>
@@ -5044,7 +5044,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D81" s="23">
         <v>2.1107940845523228</v>
@@ -5101,7 +5101,7 @@
         <v>241</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D82" s="20">
         <v>2.4399774236964356</v>
@@ -5158,7 +5158,7 @@
         <v>241001</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D83" s="20">
         <v>2.1395435640396716</v>
@@ -5215,7 +5215,7 @@
         <v>241999</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D84" s="20">
         <v>3.0013200826919726</v>
@@ -5272,7 +5272,7 @@
         <v>251</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D85" s="20">
         <v>3.1613372093023258</v>
@@ -5329,7 +5329,7 @@
         <v>252</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D86" s="20">
         <v>2.7964408934083895</v>
@@ -5386,7 +5386,7 @@
         <v>254</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D87" s="20">
         <v>3.8206547741097672</v>
@@ -5443,7 +5443,7 @@
         <v>255</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D88" s="20">
         <v>1.6894844159627147</v>
@@ -5500,7 +5500,7 @@
         <v>256</v>
       </c>
       <c r="C89" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D89" s="20">
         <v>3.5349854227405246</v>
@@ -5557,7 +5557,7 @@
         <v>257</v>
       </c>
       <c r="C90" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D90" s="20">
         <v>2.4042464612822645</v>
@@ -5614,7 +5614,7 @@
         <v>2</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D91" s="23">
         <v>2.6379068587965038</v>
@@ -5671,7 +5671,7 @@
         <v>351</v>
       </c>
       <c r="C92" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D92" s="20">
         <v>2.7418321588725174</v>
@@ -5728,7 +5728,7 @@
         <v>352</v>
       </c>
       <c r="C93" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D93" s="20">
         <v>2.1076746849942727</v>
@@ -5785,7 +5785,7 @@
         <v>353</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D94" s="20">
         <v>2.7336300063572789</v>
@@ -5842,7 +5842,7 @@
         <v>354</v>
       </c>
       <c r="C95" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D95" s="20">
         <v>0.39277297721916732</v>
@@ -5899,7 +5899,7 @@
         <v>355</v>
       </c>
       <c r="C96" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D96" s="20">
         <v>2.8538316673909896</v>
@@ -5956,7 +5956,7 @@
         <v>356</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D97" s="20">
         <v>1.4809236947791165</v>
@@ -6013,7 +6013,7 @@
         <v>357</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D98" s="20">
         <v>1.3067922808083878</v>
@@ -6070,7 +6070,7 @@
         <v>358</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D99" s="20">
         <v>2.454193982181879</v>
@@ -6127,7 +6127,7 @@
         <v>359</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D100" s="20">
         <v>3.7231384307846076</v>
@@ -6184,7 +6184,7 @@
         <v>360</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D101" s="20">
         <v>1.9023689877961234</v>
@@ -6241,7 +6241,7 @@
         <v>361</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D102" s="20">
         <v>2.6276722090261284</v>
@@ -6298,7 +6298,7 @@
         <v>3</v>
       </c>
       <c r="C103" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D103" s="23">
         <v>2.4655256443335913</v>
@@ -6355,7 +6355,7 @@
         <v>401</v>
       </c>
       <c r="C104" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D104" s="20">
         <v>2.9328988298029919</v>
@@ -6412,7 +6412,7 @@
         <v>402</v>
       </c>
       <c r="C105" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D105" s="20">
         <v>1.6888250089831118</v>
@@ -6469,7 +6469,7 @@
         <v>403</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D106" s="20">
         <v>2.4787535410764874</v>
@@ -6526,7 +6526,7 @@
         <v>404</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D107" s="20">
         <v>3.0389112770033693</v>
@@ -6583,7 +6583,7 @@
         <v>405</v>
       </c>
       <c r="C108" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D108" s="20">
         <v>4.7520124642949888</v>
@@ -6640,7 +6640,7 @@
         <v>451</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D109" s="20">
         <v>2.7676399026763989</v>
@@ -6697,7 +6697,7 @@
         <v>452</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D110" s="20">
         <v>3.7654552266766581</v>
@@ -6754,7 +6754,7 @@
         <v>453</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D111" s="20">
         <v>1.3089418072859171</v>
@@ -6811,7 +6811,7 @@
         <v>454</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D112" s="20">
         <v>1.3117099928452181</v>
@@ -6868,7 +6868,7 @@
         <v>455</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D113" s="20">
         <v>2.5761973875181421</v>
@@ -6925,7 +6925,7 @@
         <v>456</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D114" s="20">
         <v>0.85682074408117248</v>
@@ -6982,7 +6982,7 @@
         <v>457</v>
       </c>
       <c r="C115" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D115" s="20">
         <v>1.9021322288694587</v>
@@ -7039,7 +7039,7 @@
         <v>458</v>
       </c>
       <c r="C116" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D116" s="20">
         <v>2.1187427240977881</v>
@@ -7096,7 +7096,7 @@
         <v>459</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D117" s="20">
         <v>1.0180926096289482</v>
@@ -7153,7 +7153,7 @@
         <v>460</v>
       </c>
       <c r="C118" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D118" s="20">
         <v>3.2243568138411414</v>
@@ -7210,7 +7210,7 @@
         <v>461</v>
       </c>
       <c r="C119" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D119" s="20">
         <v>1.7389642652398243</v>
@@ -7267,7 +7267,7 @@
         <v>462</v>
       </c>
       <c r="C120" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D120" s="20">
         <v>2.0346646571213265</v>
@@ -7324,7 +7324,7 @@
         <v>4</v>
       </c>
       <c r="C121" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D121" s="23">
         <v>2.1221095888212016</v>
@@ -7381,7 +7381,7 @@
         <v>0</v>
       </c>
       <c r="C122" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D122" s="23">
         <v>2.358901461799491</v>
@@ -7435,7 +7435,7 @@
     <row r="123" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="24"/>
       <c r="C123" s="25" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7444,24 +7444,24 @@
     <row r="125" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="24"/>
       <c r="C125" s="26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="24"/>
       <c r="C126" s="26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="24"/>
       <c r="C127" s="26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>